<commit_message>
update edit user popup
</commit_message>
<xml_diff>
--- a/public/users.xlsx
+++ b/public/users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaree\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F37E72-D0D1-4FAE-B6E2-1AB506C11A04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{852DC60D-CFA2-4E6F-9EE9-6581137628B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{07BFC873-6D7C-4001-B48B-7B65D5328514}"/>
   </bookViews>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="63">
-  <si>
-    <t>UserName</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="74">
   <si>
     <t>Role</t>
   </si>
@@ -45,27 +42,15 @@
     <t>Email Id</t>
   </si>
   <si>
-    <t>Tenant</t>
-  </si>
-  <si>
-    <t>Sub-Tenant</t>
-  </si>
-  <si>
     <t>Last Login</t>
   </si>
   <si>
     <t>Jareen</t>
   </si>
   <si>
-    <t>Admin</t>
-  </si>
-  <si>
     <t>jareentaj.syed@algonox.com</t>
   </si>
   <si>
-    <t>Jareentaj</t>
-  </si>
-  <si>
     <t>10:34AM</t>
   </si>
   <si>
@@ -223,6 +208,54 @@
   </si>
   <si>
     <t>17/06/2024 9:38PM</t>
+  </si>
+  <si>
+    <t>User Name</t>
+  </si>
+  <si>
+    <t>Partner</t>
+  </si>
+  <si>
+    <t>Sub Partner</t>
+  </si>
+  <si>
+    <t>Altaworx</t>
+  </si>
+  <si>
+    <t>Atlantech-AWX</t>
+  </si>
+  <si>
+    <t>CSV-AWX</t>
+  </si>
+  <si>
+    <t>Frontier-AWX</t>
+  </si>
+  <si>
+    <t>GoTech-AWX</t>
+  </si>
+  <si>
+    <t>Local IT-AWX</t>
+  </si>
+  <si>
+    <t>Titanium-AWX</t>
+  </si>
+  <si>
+    <t>Castle Point-AWX</t>
+  </si>
+  <si>
+    <t>Agent</t>
+  </si>
+  <si>
+    <t>Agent Partner Admin</t>
+  </si>
+  <si>
+    <t>Super Admin</t>
+  </si>
+  <si>
+    <t>Partner Admin</t>
+  </si>
+  <si>
+    <t>User</t>
   </si>
 </sst>
 </file>
@@ -588,16 +621,16 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.77734375" customWidth="1"/>
-    <col min="2" max="2" width="14.77734375" customWidth="1"/>
+    <col min="2" max="2" width="17.77734375" customWidth="1"/>
     <col min="3" max="3" width="26.21875" customWidth="1"/>
     <col min="4" max="4" width="15.44140625" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="15.77734375" customWidth="1"/>
     <col min="6" max="6" width="13.88671875" customWidth="1"/>
     <col min="7" max="7" width="14.109375" customWidth="1"/>
     <col min="8" max="8" width="17.33203125" customWidth="1"/>
@@ -606,321 +639,321 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
       <c r="G1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="I1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>69</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="I2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="H3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="I3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
       <c r="G4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="I4" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>69</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="F5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="H5" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="I5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>72</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="F6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G6" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="H6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="I6" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>66</v>
       </c>
       <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" t="s">
         <v>15</v>
       </c>
-      <c r="G7" t="s">
-        <v>20</v>
-      </c>
       <c r="H7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="I7" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>69</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>67</v>
       </c>
       <c r="F8" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G8" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H8" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I8" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="E9" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="F9" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G9" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="H9" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="I9" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>69</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="E10" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="F10" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G10" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H10" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="I10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="E11" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="F11" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G11" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="H11" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="I11" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>